<commit_message>
Updated setting_analysis script to include additional analyses
</commit_message>
<xml_diff>
--- a/keyboard_trials.xlsx
+++ b/keyboard_trials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kburc\D1V1\Documents\!Dell64docs\Programming\py\kjb3_programs\Type_The_Bible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F625712D-47D2-4315-A5A7-CD9D156C7CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB77F285-FFB2-4701-9018-7D1AE0B111AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="21">
   <si>
     <t>1st Test</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Average WPM over last 10 races</t>
   </si>
   <si>
-    <t>Cycle order:</t>
-  </si>
-  <si>
     <t>Use for next set of tests:</t>
   </si>
   <si>
@@ -96,13 +93,10 @@
     <t>(Note: if running additional sets of tests right after the first set of tests, use the same cycle that you did previously. For instance, if running two sets of tests back to back, cycle through your switches as follows: Red Brown Black Black Brown Red Red Brown Black Black Brown Red Red Brown Black Black Brown Red Red Brown Black Black Brown Red.)</t>
   </si>
   <si>
-    <t>Red Brown Black Black Brown Red Red Brown Black Black Brown Red</t>
-  </si>
-  <si>
-    <t>Brown Black Red Red Black Brown Brown Black Red Red Black Brown</t>
-  </si>
-  <si>
-    <t>Black Red Brown Brown Red Black Black Red Brown Brown Red Black</t>
+    <t>Switches by cycle order:</t>
+  </si>
+  <si>
+    <t>A 'Y' in the columns to the left shows which cycle to do next.</t>
   </si>
 </sst>
 </file>
@@ -138,11 +132,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,24 +414,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="7" max="7" width="13.19921875" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="9" width="38.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -448,12 +441,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -473,9 +466,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <f>D2+1</f>
@@ -486,7 +479,7 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <v>152.61699999999999</v>
+        <v>140.06100000000001</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -495,9 +488,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <f>B5+10</f>
@@ -508,7 +501,7 @@
         <v>20</v>
       </c>
       <c r="D6">
-        <v>153.05699999999999</v>
+        <v>144.89599999999999</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -517,9 +510,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <f t="shared" ref="B7:B16" si="0">B6+10</f>
@@ -530,12 +523,15 @@
         <v>30</v>
       </c>
       <c r="D7">
-        <v>158.15199999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+        <v>146.749</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
@@ -546,12 +542,18 @@
         <v>40</v>
       </c>
       <c r="D8">
-        <v>136.05699999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+        <v>145.95400000000001</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
@@ -562,18 +564,21 @@
         <v>50</v>
       </c>
       <c r="D9">
-        <v>149.15700000000001</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+        <v>164.17</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
@@ -584,18 +589,21 @@
         <v>60</v>
       </c>
       <c r="D10">
-        <v>143.85599999999999</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
+        <v>150.68100000000001</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
@@ -606,21 +614,21 @@
         <v>70</v>
       </c>
       <c r="D11">
-        <v>134.34700000000001</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
+        <v>140.142</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
@@ -631,18 +639,21 @@
         <v>80</v>
       </c>
       <c r="D12">
-        <v>142.94900000000001</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
+        <v>145.62899999999999</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
@@ -653,15 +664,21 @@
         <v>90</v>
       </c>
       <c r="D13">
-        <v>139.315</v>
+        <v>144.98099999999999</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
@@ -672,12 +689,21 @@
         <v>100</v>
       </c>
       <c r="D14">
-        <v>144.334</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+        <v>154.321</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
@@ -688,12 +714,21 @@
         <v>110</v>
       </c>
       <c r="D15">
-        <v>138.36699999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+        <v>136.476</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
@@ -704,7 +739,84 @@
         <v>120</v>
       </c>
       <c r="D16">
-        <v>131.41399999999999</v>
+        <v>132.02000000000001</v>
+      </c>
+      <c r="F16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.45">
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.45">
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.45">
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.45">
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.45">
+      <c r="F21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.45">
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="5:8" x14ac:dyDescent="0.45">
+      <c r="F24" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>